<commit_message>
Merge and create playlist
</commit_message>
<xml_diff>
--- a/gantt chart.xlsx
+++ b/gantt chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Project: Shared Sounds</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Get Spotify songs</t>
+  </si>
+  <si>
+    <t>Combine songs and create playlist</t>
   </si>
   <si>
     <t>Testing</t>
@@ -268,6 +271,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -278,53 +288,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -342,13 +308,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="8" tint="-0.499984740745262"/>
       <name val="Calibri"/>
@@ -357,7 +316,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,9 +330,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -407,7 +410,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +452,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,19 +470,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,19 +506,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.349986266670736"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,19 +524,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,25 +566,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="1" tint="0.349986266670736"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,67 +596,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,58 +706,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="8"/>
-      </top>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="8" tint="0.799981688894314"/>
-      </right>
-      <top style="medium">
-        <color theme="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.349986266670736"/>
       </left>
@@ -766,6 +717,17 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.349986266670736"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,6 +758,47 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8" tint="0.799981688894314"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -807,142 +810,142 @@
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="12" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="15" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="9" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="13" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1420,8 +1423,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Milestones34" displayName="Milestones34" ref="B7:G32" totalsRowShown="0">
-  <autoFilter ref="B7:G32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Milestones34" displayName="Milestones34" ref="B7:G33" totalsRowShown="0">
+  <autoFilter ref="B7:G33">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1700,10 +1703,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EM34"/>
+  <dimension ref="A1:EM35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" showRuler="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" showRuler="0" topLeftCell="Z9" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.775" defaultRowHeight="30" customHeight="1"/>
@@ -3930,7 +3933,7 @@
         <v>45303</v>
       </c>
       <c r="F13" s="39">
-        <f t="shared" ref="F13:F21" si="12">E13+G13</f>
+        <f t="shared" ref="F13:F24" si="12">E13+G13</f>
         <v>45306</v>
       </c>
       <c r="G13" s="36">
@@ -5169,7 +5172,7 @@
         <v>45414</v>
       </c>
       <c r="F21" s="39">
-        <f>E21+G21</f>
+        <f t="shared" si="12"/>
         <v>45416</v>
       </c>
       <c r="G21" s="36">
@@ -5325,7 +5328,7 @@
         <v>45416</v>
       </c>
       <c r="F22" s="39">
-        <f>E22+G22</f>
+        <f t="shared" si="12"/>
         <v>45419</v>
       </c>
       <c r="G22" s="36">
@@ -5481,7 +5484,7 @@
         <v>45419</v>
       </c>
       <c r="F23" s="39">
-        <f>E23+G23</f>
+        <f t="shared" si="12"/>
         <v>45420</v>
       </c>
       <c r="G23" s="36">
@@ -5637,7 +5640,7 @@
         <v>45419</v>
       </c>
       <c r="F24" s="39">
-        <f>E24+G24</f>
+        <f t="shared" si="12"/>
         <v>45421</v>
       </c>
       <c r="G24" s="36">
@@ -5780,16 +5783,25 @@
       <c r="EL24" s="49"/>
       <c r="EM24" s="49"/>
     </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:143">
+    <row r="25" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
       <c r="A25" s="9"/>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
+      <c r="D25" s="24">
+        <v>1</v>
+      </c>
+      <c r="E25" s="38">
+        <v>45421</v>
+      </c>
+      <c r="F25" s="39">
+        <f>E25+G25</f>
+        <v>45423</v>
+      </c>
+      <c r="G25" s="36">
+        <v>2</v>
+      </c>
       <c r="H25" s="37"/>
       <c r="I25" s="49"/>
       <c r="J25" s="49"/>
@@ -5927,15 +5939,13 @@
       <c r="EL25" s="49"/>
       <c r="EM25" s="49"/>
     </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:143">
       <c r="A26" s="9"/>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="21"/>
-      <c r="D26" s="24">
-        <v>0</v>
-      </c>
+      <c r="D26" s="26"/>
       <c r="E26" s="38"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
@@ -6077,7 +6087,7 @@
       <c r="EM26" s="49"/>
     </row>
     <row r="27" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
-      <c r="A27" s="2"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="23" t="s">
         <v>27</v>
       </c>
@@ -6374,13 +6384,15 @@
       <c r="EL28" s="49"/>
       <c r="EM28" s="49"/>
     </row>
-    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:143">
+    <row r="29" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
       <c r="A29" s="2"/>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="23" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="26"/>
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
       <c r="E29" s="38"/>
       <c r="F29" s="36"/>
       <c r="G29" s="36"/>
@@ -6521,15 +6533,13 @@
       <c r="EL29" s="49"/>
       <c r="EM29" s="49"/>
     </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:143">
       <c r="A30" s="2"/>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="24">
-        <v>0</v>
-      </c>
+      <c r="D30" s="26"/>
       <c r="E30" s="38"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
@@ -6680,7 +6690,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
       <c r="I31" s="49"/>
@@ -6968,17 +6978,166 @@
       <c r="EL32" s="49"/>
       <c r="EM32" s="49"/>
     </row>
-    <row r="33" customHeight="1" spans="3:8">
-      <c r="C33" s="27"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="41"/>
+    <row r="33" s="1" customFormat="1" customHeight="1" outlineLevel="1" spans="1:143">
+      <c r="A33" s="2"/>
+      <c r="B33" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="49"/>
+      <c r="Z33" s="49"/>
+      <c r="AA33" s="49"/>
+      <c r="AB33" s="49"/>
+      <c r="AC33" s="49"/>
+      <c r="AD33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33" s="49"/>
+      <c r="AG33" s="49"/>
+      <c r="AH33" s="49"/>
+      <c r="AI33" s="49"/>
+      <c r="AJ33" s="49"/>
+      <c r="AK33" s="49"/>
+      <c r="AL33" s="49"/>
+      <c r="AM33" s="49"/>
+      <c r="AN33" s="49"/>
+      <c r="AO33" s="49"/>
+      <c r="AP33" s="49"/>
+      <c r="AQ33" s="49"/>
+      <c r="AR33" s="49"/>
+      <c r="AS33" s="49"/>
+      <c r="AT33" s="49"/>
+      <c r="AU33" s="49"/>
+      <c r="AV33" s="49"/>
+      <c r="AW33" s="49"/>
+      <c r="AX33" s="49"/>
+      <c r="AY33" s="49"/>
+      <c r="AZ33" s="49"/>
+      <c r="BA33" s="49"/>
+      <c r="BB33" s="49"/>
+      <c r="BC33" s="49"/>
+      <c r="BD33" s="49"/>
+      <c r="BE33" s="49"/>
+      <c r="BF33" s="49"/>
+      <c r="BG33" s="49"/>
+      <c r="BH33" s="49"/>
+      <c r="BI33" s="49"/>
+      <c r="BJ33" s="49"/>
+      <c r="BK33" s="49"/>
+      <c r="BL33" s="49"/>
+      <c r="BM33" s="49"/>
+      <c r="BN33" s="49"/>
+      <c r="BO33" s="49"/>
+      <c r="BP33" s="49"/>
+      <c r="BQ33" s="49"/>
+      <c r="BR33" s="49"/>
+      <c r="BS33" s="49"/>
+      <c r="BT33" s="49"/>
+      <c r="BU33" s="49"/>
+      <c r="BV33" s="49"/>
+      <c r="BW33" s="49"/>
+      <c r="BX33" s="49"/>
+      <c r="BY33" s="49"/>
+      <c r="BZ33" s="49"/>
+      <c r="CA33" s="49"/>
+      <c r="CB33" s="49"/>
+      <c r="CC33" s="49"/>
+      <c r="CD33" s="49"/>
+      <c r="CE33" s="49"/>
+      <c r="CF33" s="49"/>
+      <c r="CG33" s="49"/>
+      <c r="CH33" s="49"/>
+      <c r="CI33" s="49"/>
+      <c r="CJ33" s="49"/>
+      <c r="CK33" s="49"/>
+      <c r="CL33" s="49"/>
+      <c r="CM33" s="49"/>
+      <c r="CN33" s="49"/>
+      <c r="CO33" s="49"/>
+      <c r="CP33" s="49"/>
+      <c r="CQ33" s="49"/>
+      <c r="CR33" s="49"/>
+      <c r="CS33" s="49"/>
+      <c r="CT33" s="49"/>
+      <c r="CU33" s="49"/>
+      <c r="CV33" s="49"/>
+      <c r="CW33" s="49"/>
+      <c r="CX33" s="49"/>
+      <c r="CY33" s="49"/>
+      <c r="CZ33" s="49"/>
+      <c r="DA33" s="49"/>
+      <c r="DB33" s="49"/>
+      <c r="DC33" s="49"/>
+      <c r="DD33" s="49"/>
+      <c r="DE33" s="49"/>
+      <c r="DF33" s="49"/>
+      <c r="DG33" s="49"/>
+      <c r="DH33" s="49"/>
+      <c r="DI33" s="49"/>
+      <c r="DJ33" s="49"/>
+      <c r="DK33" s="49"/>
+      <c r="DL33" s="49"/>
+      <c r="DM33" s="49"/>
+      <c r="DN33" s="49"/>
+      <c r="DO33" s="49"/>
+      <c r="DP33" s="49"/>
+      <c r="DQ33" s="49"/>
+      <c r="DR33" s="49"/>
+      <c r="DS33" s="49"/>
+      <c r="DT33" s="49"/>
+      <c r="DU33" s="49"/>
+      <c r="DV33" s="49"/>
+      <c r="DW33" s="49"/>
+      <c r="DX33" s="49"/>
+      <c r="DY33" s="49"/>
+      <c r="DZ33" s="49"/>
+      <c r="EA33" s="49"/>
+      <c r="EB33" s="49"/>
+      <c r="EC33" s="49"/>
+      <c r="ED33" s="49"/>
+      <c r="EE33" s="49"/>
+      <c r="EF33" s="49"/>
+      <c r="EG33" s="49"/>
+      <c r="EH33" s="49"/>
+      <c r="EI33" s="49"/>
+      <c r="EJ33" s="49"/>
+      <c r="EK33" s="49"/>
+      <c r="EL33" s="49"/>
+      <c r="EM33" s="49"/>
     </row>
-    <row r="34" customHeight="1" spans="3:3">
-      <c r="C34" s="28"/>
+    <row r="34" customHeight="1" spans="3:8">
+      <c r="C34" s="27"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41"/>
+    </row>
+    <row r="35" customHeight="1" spans="3:3">
+      <c r="C35" s="28"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D7:D16 D18:D19 D25:D32">
+  <conditionalFormatting sqref="D7:D16 D18:D19 D26:D33">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6987,17 +7146,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{86f64265-14bf-4ef8-946b-6c441c37c5eb}</x14:id>
+          <x14:id>{6856d85f-5f0e-4cd2-8f19-98aa02889ee9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:EM16 I18:EM19 I25:EM32">
+  <conditionalFormatting sqref="I8:EM16 I18:EM19 I26:EM33">
     <cfRule type="expression" dxfId="0" priority="15" stopIfTrue="1">
       <formula>AND(I$6&gt;=$E8,I$6&lt;$E8+$G8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17 D20:D24">
+  <conditionalFormatting sqref="D17 D20:D25">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7006,12 +7165,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{dcd6b5e6-bd52-4083-a94b-3b47385559e3}</x14:id>
+          <x14:id>{fd479afc-e0e1-469b-93d6-95c5c26b6cba}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17:EM17 I20:EM24">
+  <conditionalFormatting sqref="I17:EM17 I20:EM25">
     <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
       <formula>AND(I$6&gt;=$E17,I$6&lt;$E17+$G17)</formula>
     </cfRule>
@@ -7039,7 +7198,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{dccdea09-7142-4e50-9cac-710ac466748f}">
+          <x14:cfRule type="iconSet" priority="12" id="{2d1b2535-fd15-4c80-b142-2c3bbf9c3161}">
             <x14:iconSet iconSet="3Flags" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7058,7 +7217,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{86f64265-14bf-4ef8-946b-6c441c37c5eb}">
+          <x14:cfRule type="dataBar" id="{6856d85f-5f0e-4cd2-8f19-98aa02889ee9}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -7070,10 +7229,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D16 D18:D19 D25:D32</xm:sqref>
+          <xm:sqref>D7:D16 D18:D19 D26:D33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{dcd6b5e6-bd52-4083-a94b-3b47385559e3}">
+          <x14:cfRule type="dataBar" id="{fd479afc-e0e1-469b-93d6-95c5c26b6cba}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -7085,7 +7244,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D17 D20:D24</xm:sqref>
+          <xm:sqref>D17 D20:D25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>